<commit_message>
admin authenticated services updated
</commit_message>
<xml_diff>
--- a/resources/static/assets/uploads/vouchers.xlsx
+++ b/resources/static/assets/uploads/vouchers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4761755-BAE4-42A5-987D-29EE126B84C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63B1FE5-6D3F-4DF4-8CFE-BE5AB1475162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{D691A743-7117-4F18-A715-EE7206055A6D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -48,24 +48,6 @@
     <t>234sdf</t>
   </si>
   <si>
-    <t>voucher_one</t>
-  </si>
-  <si>
-    <t>voucher_two</t>
-  </si>
-  <si>
-    <t>voucher_three</t>
-  </si>
-  <si>
-    <t>voucher_four</t>
-  </si>
-  <si>
-    <t>voucher_five</t>
-  </si>
-  <si>
-    <t>voucher_six</t>
-  </si>
-  <si>
     <t>asd123</t>
   </si>
   <si>
@@ -90,28 +72,31 @@
     <t>expiry_date</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>fgfg</t>
-  </si>
-  <si>
-    <t>hygff</t>
-  </si>
-  <si>
-    <t>hygh</t>
-  </si>
-  <si>
-    <t>hgff</t>
-  </si>
-  <si>
-    <t>grg</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>rr</t>
+    <t>Burger King</t>
+  </si>
+  <si>
+    <t>Zamber</t>
+  </si>
+  <si>
+    <t>Renee</t>
+  </si>
+  <si>
+    <t>Yatra</t>
+  </si>
+  <si>
+    <t>Ibibo</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>cosmetics</t>
+  </si>
+  <si>
+    <t>dining</t>
   </si>
 </sst>
 </file>
@@ -467,7 +452,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,19 +465,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -500,19 +485,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>250</v>
       </c>
       <c r="F2" s="1">
-        <v>45175</v>
+        <v>45178</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -520,19 +505,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>300</v>
       </c>
       <c r="F3" s="1">
-        <v>45175</v>
+        <v>45178</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -540,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -548,11 +533,11 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
+      <c r="E4">
+        <v>269</v>
       </c>
       <c r="F4" s="1">
-        <v>45175</v>
+        <v>45179</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -560,19 +545,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>200</v>
       </c>
       <c r="F5" s="1">
-        <v>45175</v>
+        <v>45177</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -580,19 +565,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>199</v>
       </c>
       <c r="F6" s="1">
-        <v>45175</v>
+        <v>45178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -600,19 +585,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>299</v>
       </c>
       <c r="F7" s="1">
-        <v>45175</v>
+        <v>45177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>